<commit_message>
Identify root cause of Line template loading failure
## Root Cause
Line template uses simplified property format incompatible with OrcaFlex 11.5e.
Lines require array-based format for connections and properties.

## Testing Evidence
- ✅ LineTypes file (06_line_types.yml) loads successfully
- ✅ Master file loads up to LineTypes inclusion
- ❌ Master file fails when Lines (07_lines.yml) added
- Error: "Failed to set LineType[0]=MooringChain (invalid index)"

## Format Mismatch Identified
Current (simplified - doesn't work):

Required (array-based - from reference):

## Next Steps
1. Update _07_lines_data.yml.j2 to use array-based format
2. Match reference file structure from _07_lines.yml
3. Test loading with corrected format

## Progress
- Wrapper template system: 100% ✅
- Core validation: 22% (2/9 files) ✅
- Root cause analysis: Complete ✅

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/projects/modules/calm/baltic_039m/TEST_OPERABILITY/results/project_summary.xlsx
+++ b/projects/modules/calm/baltic_039m/TEST_OPERABILITY/results/project_summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\workspace-hub\digitalmodel\projects\modules\calm\baltic_039m\TEST_OPERABILITY\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Acma-ansys05\d\workspace-hub\digitalmodel\projects\modules\calm\baltic_039m\TEST_OPERABILITY\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F886EA48-0B58-4C8F-90EB-70DAB4613732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191C9218-AE93-4124-90AD-39634FC039A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2410E4D2-3E22-45C0-A70E-D969989C64D5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2410E4D2-3E22-45C0-A70E-D969989C64D5}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="113">
   <si>
     <t>fe_filename</t>
   </si>
@@ -294,27 +294,6 @@
     <t>kN</t>
   </si>
   <si>
-    <t>Mooring 1</t>
-  </si>
-  <si>
-    <t>Mooring 2</t>
-  </si>
-  <si>
-    <t>Mooring 3</t>
-  </si>
-  <si>
-    <t>Mooring 4</t>
-  </si>
-  <si>
-    <t>Mooring 5</t>
-  </si>
-  <si>
-    <t>Mooring 6</t>
-  </si>
-  <si>
-    <t>CALM Buoy - Chain Maximum Tension</t>
-  </si>
-  <si>
     <t>Hawser Maximum Tension</t>
   </si>
   <si>
@@ -355,6 +334,48 @@
   </si>
   <si>
     <t>Summary Results</t>
+  </si>
+  <si>
+    <t>Line 1</t>
+  </si>
+  <si>
+    <t>Line 2</t>
+  </si>
+  <si>
+    <t>Line 3</t>
+  </si>
+  <si>
+    <t>Line 4</t>
+  </si>
+  <si>
+    <t>Line 5</t>
+  </si>
+  <si>
+    <t>Line 6</t>
+  </si>
+  <si>
+    <t>Mooring Line Tension</t>
+  </si>
+  <si>
+    <t>Alan C. McClure Associates, Inc.</t>
+  </si>
+  <si>
+    <t>Drilling Island - SPM Export Terminal Mooring Analysis</t>
+  </si>
+  <si>
+    <t>ACMA Job No. B1535_1</t>
+  </si>
+  <si>
+    <t>November 14, 20025</t>
+  </si>
+  <si>
+    <t>0 deg colinear (kN)</t>
+  </si>
+  <si>
+    <t>30 deg colinear (kN)</t>
+  </si>
+  <si>
+    <t>DHI - Drilling Island Development Project</t>
   </si>
 </sst>
 </file>
@@ -364,13 +385,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -547,6 +574,20 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -734,12 +775,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE7F0F2"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -869,90 +910,186 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1018,14 +1155,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1378,214 +1515,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83C9466-28DC-4F9A-8119-8ADCD4B271B4}">
-  <dimension ref="A2:D24"/>
+  <dimension ref="B1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4"/>
-    <col min="2" max="2" width="24.77734375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="4"/>
-    <col min="4" max="4" width="17.6640625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="2.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="3"/>
+    <col min="4" max="4" width="17.6640625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="2:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B1" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="22.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="17" t="s">
+    <row r="9" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D12" s="6">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="17" t="s">
+    <row r="14" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D16" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+    <row r="17" spans="2:4" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D17" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="17" t="s">
+    <row r="19" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="7">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B20" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B25" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D27" s="6">
         <v>2.5</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D28" s="6">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D29" s="6">
         <v>1.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B4:D4"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B25:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1594,571 +1754,669 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4A4F7C-0E34-4C76-8355-3E925DD5DDC3}">
-  <dimension ref="A2:O23"/>
+  <dimension ref="B1:O27"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4"/>
-    <col min="2" max="2" width="24.77734375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="4"/>
-    <col min="4" max="14" width="9" style="4" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="2.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="3"/>
+    <col min="4" max="14" width="9" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="17" t="s">
+    <row r="1" spans="2:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B1" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="22.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B8" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="N8" s="32"/>
+      <c r="O8" s="31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="12">
-        <f>lines!I2</f>
-        <v>34.085662999999997</v>
-      </c>
-      <c r="E6" s="12">
-        <f>lines!K2</f>
-        <v>10.742940000000001</v>
-      </c>
-      <c r="F6" s="12">
-        <f>lines!M2</f>
-        <v>14.269387999999999</v>
-      </c>
-      <c r="G6" s="12">
-        <f>lines!O2</f>
-        <v>864.59484899999995</v>
-      </c>
-      <c r="H6" s="12">
-        <f>lines!Q2</f>
-        <v>811.29107699999997</v>
-      </c>
-      <c r="I6" s="12">
-        <f>lines!S2</f>
-        <v>36.235283000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="12">
-        <f>lines!I4</f>
-        <v>30.492628</v>
-      </c>
-      <c r="E7" s="12">
-        <f>lines!K4</f>
-        <v>11.070611</v>
-      </c>
-      <c r="F7" s="12">
-        <f>lines!M4</f>
-        <v>10.540855000000001</v>
-      </c>
-      <c r="G7" s="12">
-        <f>lines!O4</f>
-        <v>512.41156000000001</v>
-      </c>
-      <c r="H7" s="13">
-        <f>lines!Q4</f>
-        <v>2267.6857909999999</v>
-      </c>
-      <c r="I7" s="12">
-        <f>lines!S4</f>
-        <v>995.96636999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="B9" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="14" t="str">
-        <f t="shared" ref="E10:N10" si="0">C10</f>
+      <c r="E9" s="31" t="str">
+        <f t="shared" ref="E9:N9" si="0">C9</f>
         <v>Min</v>
       </c>
-      <c r="F10" s="14" t="str">
+      <c r="F9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Max</v>
       </c>
-      <c r="G10" s="14" t="str">
+      <c r="G9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Min</v>
       </c>
-      <c r="H10" s="14" t="str">
+      <c r="H9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Max</v>
       </c>
-      <c r="I10" s="14" t="str">
+      <c r="I9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Min</v>
       </c>
-      <c r="J10" s="14" t="str">
+      <c r="J9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Max</v>
       </c>
-      <c r="K10" s="14" t="str">
+      <c r="K9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Min</v>
       </c>
-      <c r="L10" s="14" t="str">
+      <c r="L9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Max</v>
       </c>
-      <c r="M10" s="14" t="str">
+      <c r="M9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Min</v>
       </c>
-      <c r="N10" s="14" t="str">
+      <c r="N9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Max</v>
       </c>
-      <c r="O10" s="14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="O9" s="31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C10" s="10">
         <f>buoy!H2</f>
         <v>-4.219525</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D10" s="10">
         <f>buoy!I2</f>
         <v>5.9944670000000002</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E10" s="10">
         <f>buoy!J2</f>
         <v>2.4569000000000001</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F10" s="10">
         <f>buoy!K2</f>
         <v>5.0679850000000002</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G10" s="10">
         <f>buoy!L2</f>
         <v>4.4764999999999999E-2</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H10" s="10">
         <f>buoy!M2</f>
         <v>2.5348639999999998</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I10" s="10">
         <f>buoy!N2</f>
         <v>-9.1503340000000009</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J10" s="10">
         <f>buoy!O2</f>
         <v>0.27551199999999998</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K10" s="10">
         <f>buoy!P2</f>
         <v>-13.648834000000001</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L10" s="10">
         <f>buoy!Q2</f>
         <v>16.285311</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="N10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="O11" s="10">
-        <f>SQRT(SUMSQ(MAX(ABS(C11),ABS(D11)),MAX(ABS(E11),ABS(F11))))</f>
+      <c r="O10" s="34">
+        <f>SQRT(SUMSQ(MAX(ABS(C10),ABS(D10)),MAX(ABS(E10),ABS(F10))))</f>
         <v>7.849720158981083</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+    <row r="11" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C11" s="10">
         <f>buoy!H4</f>
         <v>-3.932572</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D11" s="10">
         <f>buoy!I4</f>
         <v>5.5948060000000002</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E11" s="10">
         <f>buoy!J4</f>
         <v>2.28586</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F11" s="10">
         <f>buoy!K4</f>
         <v>7.5194710000000002</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G11" s="10">
         <f>buoy!L4</f>
         <v>0.107352</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H11" s="10">
         <f>buoy!M4</f>
         <v>2.3280110000000001</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I11" s="10">
         <f>buoy!N4</f>
         <v>-12.996532999999999</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J11" s="10">
         <f>buoy!O4</f>
         <v>5.3467830000000003</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K11" s="10">
         <f>buoy!P4</f>
         <v>-11.992941999999999</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L11" s="10">
         <f>buoy!Q4</f>
         <v>15.245862000000001</v>
       </c>
-      <c r="M12" s="11" t="s">
+      <c r="M11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="N12" s="11" t="s">
+      <c r="N11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="O12" s="10">
-        <f>SQRT(SUMSQ(MAX(ABS(C12),ABS(D12)),MAX(ABS(E12),ABS(F12))))</f>
+      <c r="O11" s="34">
+        <f>SQRT(SUMSQ(MAX(ABS(C11),ABS(D11)),MAX(ABS(E11),ABS(F11))))</f>
         <v>9.3725289168653401</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="17" t="s">
+    <row r="12" spans="2:15" ht="22.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:15" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="30"/>
+      <c r="G13" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="28"/>
+      <c r="I13" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" s="30"/>
+      <c r="K13" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" s="28"/>
+      <c r="M13" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="N13" s="30"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="D14" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="31" t="str">
+        <f t="shared" ref="E14" si="1">C14</f>
+        <v>Min</v>
+      </c>
+      <c r="F14" s="31" t="str">
+        <f t="shared" ref="F14" si="2">D14</f>
+        <v>Max</v>
+      </c>
+      <c r="G14" s="31" t="str">
+        <f t="shared" ref="G14" si="3">E14</f>
+        <v>Min</v>
+      </c>
+      <c r="H14" s="31" t="str">
+        <f t="shared" ref="H14" si="4">F14</f>
+        <v>Max</v>
+      </c>
+      <c r="I14" s="31" t="str">
+        <f t="shared" ref="I14" si="5">G14</f>
+        <v>Min</v>
+      </c>
+      <c r="J14" s="31" t="str">
+        <f t="shared" ref="J14" si="6">H14</f>
+        <v>Max</v>
+      </c>
+      <c r="K14" s="31" t="str">
+        <f t="shared" ref="K14" si="7">I14</f>
+        <v>Min</v>
+      </c>
+      <c r="L14" s="31" t="str">
+        <f t="shared" ref="L14" si="8">J14</f>
+        <v>Max</v>
+      </c>
+      <c r="M14" s="31" t="str">
+        <f t="shared" ref="M14" si="9">K14</f>
+        <v>Min</v>
+      </c>
+      <c r="N14" s="31" t="str">
+        <f t="shared" ref="N14" si="10">L14</f>
+        <v>Max</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="27">
+        <v>0.77114400000000005</v>
+      </c>
+      <c r="D15" s="27">
+        <v>34.085662999999997</v>
+      </c>
+      <c r="E15" s="27">
+        <v>3.1370209999999998</v>
+      </c>
+      <c r="F15" s="27">
+        <v>10.742940000000001</v>
+      </c>
+      <c r="G15" s="27">
+        <v>3.5280610000000001</v>
+      </c>
+      <c r="H15" s="27">
+        <v>14.269387999999999</v>
+      </c>
+      <c r="I15" s="27">
+        <v>1.9904550000000001</v>
+      </c>
+      <c r="J15" s="27">
+        <v>864.59484899999995</v>
+      </c>
+      <c r="K15" s="27">
+        <v>4.2718350000000003</v>
+      </c>
+      <c r="L15" s="27">
+        <v>811.29107699999997</v>
+      </c>
+      <c r="M15" s="27">
+        <v>4.214645</v>
+      </c>
+      <c r="N15" s="27">
+        <v>36.235283000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="27">
+        <v>1.3289820000000001</v>
+      </c>
+      <c r="D16" s="27">
+        <v>30.492628</v>
+      </c>
+      <c r="E16" s="27">
+        <v>1.533766</v>
+      </c>
+      <c r="F16" s="27">
+        <v>11.070611</v>
+      </c>
+      <c r="G16" s="27">
+        <v>4.0397369999999997</v>
+      </c>
+      <c r="H16" s="27">
+        <v>10.540855000000001</v>
+      </c>
+      <c r="I16" s="27">
+        <v>2.6165099999999999</v>
+      </c>
+      <c r="J16" s="27">
+        <v>512.41156000000001</v>
+      </c>
+      <c r="K16" s="27">
+        <v>0.86419999999999997</v>
+      </c>
+      <c r="L16" s="27">
+        <v>2267.6857909999999</v>
+      </c>
+      <c r="M16" s="27">
+        <v>5.9883179999999996</v>
+      </c>
+      <c r="N16" s="27">
+        <v>995.96636999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" ht="19.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:14" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+    <row r="20" spans="2:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D20" s="11">
         <f>lines!U2</f>
         <v>150.64286799999999</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
+    <row r="21" spans="2:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D21" s="11">
         <f>lines!U4</f>
         <v>196.693085</v>
       </c>
     </row>
-    <row r="19" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="18" t="s">
+    <row r="22" spans="2:14" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="N23" s="32"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="N19" s="18"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E20" s="14" t="str">
-        <f t="shared" ref="E20" si="1">C20</f>
+      <c r="E24" s="31" t="str">
+        <f t="shared" ref="E24" si="11">C24</f>
         <v>Min</v>
       </c>
-      <c r="F20" s="14" t="str">
-        <f t="shared" ref="F20" si="2">D20</f>
+      <c r="F24" s="31" t="str">
+        <f t="shared" ref="F24" si="12">D24</f>
         <v>Max</v>
       </c>
-      <c r="G20" s="14" t="str">
-        <f t="shared" ref="G20" si="3">E20</f>
+      <c r="G24" s="31" t="str">
+        <f t="shared" ref="G24" si="13">E24</f>
         <v>Min</v>
       </c>
-      <c r="H20" s="14" t="str">
-        <f t="shared" ref="H20" si="4">F20</f>
+      <c r="H24" s="31" t="str">
+        <f t="shared" ref="H24" si="14">F24</f>
         <v>Max</v>
       </c>
-      <c r="I20" s="14" t="str">
-        <f t="shared" ref="I20" si="5">G20</f>
+      <c r="I24" s="31" t="str">
+        <f t="shared" ref="I24" si="15">G24</f>
         <v>Min</v>
       </c>
-      <c r="J20" s="14" t="str">
-        <f t="shared" ref="J20" si="6">H20</f>
+      <c r="J24" s="31" t="str">
+        <f t="shared" ref="J24" si="16">H24</f>
         <v>Max</v>
       </c>
-      <c r="K20" s="14" t="str">
-        <f t="shared" ref="K20" si="7">I20</f>
+      <c r="K24" s="31" t="str">
+        <f t="shared" ref="K24" si="17">I24</f>
         <v>Min</v>
       </c>
-      <c r="L20" s="14" t="str">
-        <f t="shared" ref="L20" si="8">J20</f>
+      <c r="L24" s="31" t="str">
+        <f t="shared" ref="L24" si="18">J24</f>
         <v>Max</v>
       </c>
-      <c r="M20" s="14" t="str">
-        <f t="shared" ref="M20" si="9">K20</f>
+      <c r="M24" s="31" t="str">
+        <f t="shared" ref="M24" si="19">K24</f>
         <v>Min</v>
       </c>
-      <c r="N20" s="14" t="str">
-        <f t="shared" ref="N20" si="10">L20</f>
+      <c r="N24" s="31" t="str">
+        <f t="shared" ref="N24" si="20">L24</f>
         <v>Max</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
+    <row r="25" spans="2:14" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" s="11">
+      <c r="C25" s="10">
+        <f>vessel_abs!H2</f>
+        <v>-53.116329</v>
+      </c>
+      <c r="D25" s="10">
+        <f>vessel_abs!I2</f>
+        <v>93.038833999999994</v>
+      </c>
+      <c r="E25" s="10">
+        <f>vessel_abs!J2</f>
+        <v>54.544998</v>
+      </c>
+      <c r="F25" s="10">
+        <f>vessel_abs!K2</f>
+        <v>95.151038999999997</v>
+      </c>
+      <c r="G25" s="9">
         <f>vessel_abs!L2</f>
         <v>-0.67205499999999996</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H25" s="9">
         <f>vessel_abs!M2</f>
         <v>0.62917800000000002</v>
       </c>
-      <c r="I21" s="11">
+      <c r="I25" s="9">
         <f>vessel_abs!N2</f>
         <v>-8.8760049999999993</v>
       </c>
-      <c r="J21" s="11">
+      <c r="J25" s="9">
         <f>vessel_abs!O2</f>
         <v>5.384646</v>
       </c>
-      <c r="K21" s="11">
+      <c r="K25" s="9">
         <f>vessel_abs!P2</f>
         <v>-1.5783609999999999</v>
       </c>
-      <c r="L21" s="11">
+      <c r="L25" s="9">
         <f>vessel_abs!Q2</f>
         <v>1.7673380000000001</v>
       </c>
-      <c r="M21" s="11" t="s">
+      <c r="M25" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="N21" s="11" t="s">
+      <c r="N25" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+    <row r="26" spans="2:14" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="11">
+      <c r="C26" s="10">
+        <f>vessel_abs!H4</f>
+        <v>-53.528500000000001</v>
+      </c>
+      <c r="D26" s="10">
+        <f>vessel_abs!I4</f>
+        <v>82.012550000000005</v>
+      </c>
+      <c r="E26" s="10">
+        <f>vessel_abs!J4</f>
+        <v>53.746448999999998</v>
+      </c>
+      <c r="F26" s="10">
+        <f>vessel_abs!K4</f>
+        <v>106.63814499999999</v>
+      </c>
+      <c r="G26" s="9">
         <f>vessel_abs!L3</f>
         <v>-0.56144499999999997</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H26" s="9">
         <f>vessel_abs!M3</f>
         <v>0.539022</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I26" s="9">
         <f>vessel_abs!N3</f>
         <v>-5.675287</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J26" s="9">
         <f>vessel_abs!O3</f>
         <v>5.2675340000000004</v>
       </c>
-      <c r="K22" s="11">
+      <c r="K26" s="9">
         <f>vessel_abs!P3</f>
         <v>-1.485762</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L26" s="9">
         <f>vessel_abs!Q3</f>
         <v>1.602438</v>
       </c>
-      <c r="M22" s="11" t="s">
+      <c r="M26" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="N22" s="11" t="s">
+      <c r="N26" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
+    <row r="27" spans="2:14" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
+  <mergeCells count="13">
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
   </mergeCells>
-  <phoneticPr fontId="23" type="noConversion"/>
+  <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2168,12 +2426,18 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="H4" sqref="H4:S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="34.21875" customWidth="1"/>
+    <col min="3" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="19" width="12.44140625" customWidth="1"/>
+    <col min="20" max="21" width="17.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2195,50 +2459,50 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2254,50 +2518,50 @@
       <c r="E2">
         <v>100</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="18">
         <v>0.77114400000000005</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="16">
         <v>34.085662999999997</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="18">
         <v>3.1370209999999998</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="16">
         <v>10.742940000000001</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="18">
         <v>3.5280610000000001</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="16">
         <v>14.269387999999999</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="18">
         <v>1.9904550000000001</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="16">
         <v>864.59484899999995</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="18">
         <v>4.2718350000000003</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="16">
         <v>811.29107699999997</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="18">
         <v>4.214645</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="16">
         <v>36.235283000000003</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="18">
         <v>0.10661900000000001</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="16">
         <v>150.64286799999999</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2313,50 +2577,50 @@
       <c r="E3">
         <v>100</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="18">
         <v>10.975854999999999</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="16">
         <v>33.541046000000001</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="18">
         <v>6.406301</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="16">
         <v>8.4165159999999997</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="18">
         <v>3.6179999999999999</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="16">
         <v>12.686366</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="18">
         <v>3.7364489999999999</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="16">
         <v>10.779612999999999</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="18">
         <v>6.9577720000000003</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="16">
         <v>10.535887000000001</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="18">
         <v>17.881166</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="16">
         <v>33.926495000000003</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="18">
         <v>0.15807599999999999</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="16">
         <v>1.2379640000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2372,50 +2636,50 @@
       <c r="E4">
         <v>100</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="18">
         <v>1.3289820000000001</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="16">
         <v>30.492628</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="18">
         <v>1.533766</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="16">
         <v>11.070611</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="18">
         <v>4.0397369999999997</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="16">
         <v>10.540855000000001</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="18">
         <v>2.6165099999999999</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="16">
         <v>512.41156000000001</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="18">
         <v>0.86419999999999997</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="16">
         <v>2267.6857909999999</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="18">
         <v>5.9883179999999996</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="16">
         <v>995.96636999999998</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="18">
         <v>-5.6400000000000005E-4</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="16">
         <v>196.693085</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -2431,50 +2695,50 @@
       <c r="E5">
         <v>100</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="18">
         <v>1.0139910000000001</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="16">
         <v>34.506461999999999</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="18">
         <v>3.149092</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="16">
         <v>10.5901</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="18">
         <v>1.7455369999999999</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="16">
         <v>13.501179</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="18">
         <v>0.29515599999999997</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="16">
         <v>180.69757100000001</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="18">
         <v>4.2566680000000003</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="16">
         <v>1058.7113039999999</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="18">
         <v>4.4716230000000001</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="16">
         <v>37.608947999999998</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="18">
         <v>0.11720899999999999</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="16">
         <v>120.571236</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -2490,50 +2754,50 @@
       <c r="E6">
         <v>100</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="18">
         <v>10.967392</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="16">
         <v>33.541054000000003</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="18">
         <v>6.4243980000000001</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="16">
         <v>8.4165159999999997</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="18">
         <v>4.8132270000000004</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="16">
         <v>11.877186999999999</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="18">
         <v>5.1232610000000003</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="16">
         <v>9.8102619999999998</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="18">
         <v>6.9578199999999999</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="16">
         <v>10.534891999999999</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="18">
         <v>17.902376</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="16">
         <v>33.926498000000002</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="18">
         <v>0.16009499999999999</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="16">
         <v>1.237965</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -2549,46 +2813,46 @@
       <c r="E7">
         <v>100</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="18">
         <v>1.6222760000000001</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="16">
         <v>30.453878</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="18">
         <v>1.9586650000000001</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="16">
         <v>11.225820000000001</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="18">
         <v>3.9381719999999998</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="16">
         <v>9.1786019999999997</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="18">
         <v>1.5258560000000001</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="16">
         <v>21.974678000000001</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="18">
         <v>0.49963999999999997</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="16">
         <v>976.581726</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="18">
         <v>10.170781</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="16">
         <v>669.33526600000005</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="18">
         <v>4.8389000000000001E-2</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="16">
         <v>119.84232299999999</v>
       </c>
     </row>
@@ -2599,15 +2863,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDED428-B7EB-4BFE-B839-366D113A6811}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" style="21" customWidth="1"/>
+    <col min="9" max="10" width="11" style="21" customWidth="1"/>
+    <col min="11" max="12" width="10.6640625" style="21" customWidth="1"/>
+    <col min="13" max="13" width="11" style="21" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" style="21" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" style="21" customWidth="1"/>
+    <col min="16" max="16" width="11.44140625" style="21" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" style="21" customWidth="1"/>
+    <col min="18" max="18" width="11.77734375" style="21" customWidth="1"/>
+    <col min="19" max="19" width="11.5546875" style="21" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2629,44 +2907,45 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="19" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T1" s="15"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2682,44 +2961,44 @@
       <c r="E2">
         <v>100</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="18">
         <v>-4.219525</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="16">
         <v>5.9944670000000002</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="18">
         <v>2.4569000000000001</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="16">
         <v>5.0679850000000002</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="18">
         <v>4.4764999999999999E-2</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="16">
         <v>2.5348639999999998</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="18">
         <v>-9.1503340000000009</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="16">
         <v>0.27551199999999998</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="18">
         <v>-13.648834000000001</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="16">
         <v>16.285311</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="18">
         <v>-104.89180899999999</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="16">
         <v>-12.041886999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2735,44 +3014,44 @@
       <c r="E3">
         <v>100</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="18">
         <v>-4.4047080000000003</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="16">
         <v>-1.6133729999999999</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="18">
         <v>2.3943620000000001</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="16">
         <v>2.748421</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="18">
         <v>0.53306399999999998</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="16">
         <v>2.288856</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="18">
         <v>-2.3760080000000001</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="16">
         <v>-0.40455000000000002</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="18">
         <v>-9.4651130000000006</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="16">
         <v>8.4929729999999992</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="18">
         <v>-47.105638999999996</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="16">
         <v>-6.4825489999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2788,44 +3067,44 @@
       <c r="E4">
         <v>100</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="18">
         <v>-3.932572</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="16">
         <v>5.5948060000000002</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="18">
         <v>2.28586</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="16">
         <v>7.5194710000000002</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="18">
         <v>0.107352</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="16">
         <v>2.3280110000000001</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="18">
         <v>-12.996532999999999</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="16">
         <v>5.3467830000000003</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="18">
         <v>-11.992941999999999</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="16">
         <v>15.245862000000001</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="18">
         <v>-117.436893</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="16">
         <v>-14.424758000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -2841,44 +3120,44 @@
       <c r="E5">
         <v>100</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="18">
         <v>-4.1649190000000003</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="16">
         <v>5.4591479999999999</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="18">
         <v>2.523174</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="16">
         <v>5.6841049999999997</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="18">
         <v>-3.6746000000000001E-2</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="16">
         <v>2.4634149999999999</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="18">
         <v>-10.917809</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="16">
         <v>2.0371779999999999</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="18">
         <v>-13.588663</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="16">
         <v>19.038170000000001</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="18">
         <v>-81.424345000000002</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="16">
         <v>-7.8559710000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -2894,44 +3173,44 @@
       <c r="E6">
         <v>100</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="18">
         <v>-4.4047090000000004</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="16">
         <v>-1.610965</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="18">
         <v>2.3943620000000001</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="16">
         <v>2.7491310000000002</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="18">
         <v>0.53313299999999997</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="16">
         <v>2.2886479999999998</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="18">
         <v>-2.3787180000000001</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="16">
         <v>-0.40082000000000001</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="18">
         <v>-9.4642370000000007</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="16">
         <v>8.4951600000000003</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="18">
         <v>-47.60633</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="16">
         <v>-6.4826119999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -2947,40 +3226,40 @@
       <c r="E7">
         <v>100</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="18">
         <v>-3.8857629999999999</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="16">
         <v>3.1953290000000001</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="18">
         <v>2.5109590000000002</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="16">
         <v>7.1783729999999997</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="18">
         <v>6.2178999999999998E-2</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="16">
         <v>2.4874849999999999</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="18">
         <v>-13.005087</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="16">
         <v>4.9260599999999997</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="18">
         <v>-12.403962</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="16">
         <v>14.950039</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="18">
         <v>-79.851257000000004</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="16">
         <v>-5.9368689999999997</v>
       </c>
     </row>
@@ -2991,15 +3270,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA3F6D7-658C-47AF-8528-0700A529A6B0}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="35.5546875" customWidth="1"/>
+    <col min="3" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" customWidth="1"/>
+    <col min="18" max="18" width="10.77734375" customWidth="1"/>
+    <col min="19" max="19" width="10.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3021,44 +3316,45 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T1" s="15"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3074,44 +3370,44 @@
       <c r="E2">
         <v>100</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="18">
         <v>-53.116329</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="16">
         <v>93.038833999999994</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="18">
         <v>54.544998</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="16">
         <v>95.151038999999997</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="18">
         <v>-0.67205499999999996</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="16">
         <v>0.62917800000000002</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="18">
         <v>-8.8760049999999993</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="16">
         <v>5.384646</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="18">
         <v>-1.5783609999999999</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="16">
         <v>1.7673380000000001</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="18">
         <v>-153.746206</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="16">
         <v>-55.411614</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -3127,44 +3423,44 @@
       <c r="E3">
         <v>100</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="18">
         <v>-55.721977000000003</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="16">
         <v>-30.667573999999998</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="18">
         <v>79.281807000000001</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="16">
         <v>80.489845000000003</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="18">
         <v>-0.56144499999999997</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="16">
         <v>0.539022</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="18">
         <v>-5.675287</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="16">
         <v>5.2675340000000004</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="18">
         <v>-1.485762</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="16">
         <v>1.602438</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="18">
         <v>-56.501114000000001</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="16">
         <v>-53.327897</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -3180,44 +3476,44 @@
       <c r="E4">
         <v>100</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="18">
         <v>-53.528500000000001</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="16">
         <v>82.012550000000005</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="18">
         <v>53.746448999999998</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="16">
         <v>106.63814499999999</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="18">
         <v>-1.042381</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="16">
         <v>0.98170199999999996</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="18">
         <v>-16.965600999999999</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="16">
         <v>15.496741</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="18">
         <v>-2.3332389999999998</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="16">
         <v>1.9974700000000001</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="18">
         <v>-131.362078</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="16">
         <v>-54.921557999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -3233,44 +3529,44 @@
       <c r="E5">
         <v>100</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="18">
         <v>-55.068821</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="16">
         <v>27.820371999999999</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="18">
         <v>79.913048000000003</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="16">
         <v>92.829491000000004</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="18">
         <v>-0.60882499999999995</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="16">
         <v>0.65242100000000003</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="18">
         <v>-7.2702159999999996</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="16">
         <v>6.0909240000000002</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="18">
         <v>-2.3099240000000001</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="16">
         <v>2.3890359999999999</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="18">
         <v>-89.673192</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="16">
         <v>-54.863781000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -3286,44 +3582,44 @@
       <c r="E6">
         <v>100</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="18">
         <v>-55.721972999999998</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="16">
         <v>-30.109489</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="18">
         <v>79.282234000000003</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="16">
         <v>80.673820000000006</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="18">
         <v>-0.56144400000000005</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="16">
         <v>0.53902099999999997</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="18">
         <v>-5.7141869999999999</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="16">
         <v>5.2931350000000004</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="18">
         <v>-1.4857530000000001</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="16">
         <v>1.6024339999999999</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="18">
         <v>-56.649521</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="16">
         <v>-53.324103000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -3339,58 +3635,58 @@
       <c r="E7">
         <v>100</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="18">
         <v>-55.616703000000001</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="16">
         <v>46.376724000000003</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="18">
         <v>80.087547000000001</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="16">
         <v>98.498626999999999</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="18">
         <v>-1.3950849999999999</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="16">
         <v>1.499576</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="18">
         <v>-14.069989</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="16">
         <v>13.213725</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="18">
         <v>-1.0299659999999999</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="16">
         <v>1.053007</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="18">
         <v>-114.021744</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="16">
         <v>-54.416246999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>